<commit_message>
fix correçoes tab-orcamento, upload OC, ocorrencia
</commit_message>
<xml_diff>
--- a/pdf/cotacao.xlsx
+++ b/pdf/cotacao.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>PLANILHA DE COTAÇÃO</t>
   </si>
@@ -26,13 +26,16 @@
     <t>Valor unitario</t>
   </si>
   <si>
-    <t>PLACA DE IDENTIFICAÇÃO DE OBRA</t>
-  </si>
-  <si>
-    <t>LÂMPADA INCANDESCENTE (POTÊNCIA: 40 W / TENSÃO: 220 V / TIPO DE ROSCA: E-27)</t>
-  </si>
-  <si>
-    <t>LAPIS PARA CARPINTEIRO</t>
+    <t>BLOCO DE CONCRETO DE VEDAÇÃO - BLOCO INTEIRO 14 X 19 X 19 - RESISTÊNICA 3,0 MPA (ALTURA: 190 MM / COMPRIMENTO: 390 MM / LARGURA: 190 MM)</t>
+  </si>
+  <si>
+    <t>BLOCO DE CONCRETO PARA PAVIMENTAÇÃO INTERTRAVADA RETANGULAR - TRÁFEGO PESADO (COMPRIMENTO: 100 MM / ESPESSURA: 60 MM / LARGURA: 200 MM)</t>
+  </si>
+  <si>
+    <t>PEDRA BRITADA 2</t>
+  </si>
+  <si>
+    <t>CIMENTO PORTLAND CP II-Z-32 (RESISTÊNCIA: 32,00 MPA)</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,6 +493,11 @@
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>